<commit_message>
metodos de substituicao de fronteira
</commit_message>
<xml_diff>
--- a/saida.xlsx
+++ b/saida.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,122 +447,247 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>0.1288322815721658</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>0.2657586058018112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>0.4193815332872734</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>0.5993526087583387</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2.59557226510638</v>
+        <v>-0.4434531441505186</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2.291699407031611</v>
+        <v>-0.4434531441505186</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2.084974792493151</v>
+        <v>-0.6013775875253951</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.88882075758612</v>
+        <v>-0.4743415942963839</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.61170966478293</v>
+        <v>-0.4743415942963839</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5.600859562305712</v>
+        <v>0.001834528240272033</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5.135722854093962</v>
+        <v>0.001834528240272033</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>4.732931906553064</v>
+        <v>0.2473474482405971</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>4.325787756649211</v>
+        <v>0.1063814174549735</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3.896127258004254</v>
+        <v>0.1063814174549735</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>9.07455385329242</v>
+        <v>-0.02285419592424004</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>8.437778054930412</v>
+        <v>-0.02285419592424004</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>7.837253946860164</v>
+        <v>0.08759328731672891</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>7.21159509175535</v>
+        <v>0.188609191195769</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>6.619030469740215</v>
+        <v>0.188609191195769</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>9.07455385329242</v>
+        <v>-0.02285419592424004</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>8.437778054930412</v>
+        <v>-0.02285419592424004</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>7.837253946860164</v>
+        <v>0.08759328731672891</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>7.21159509175535</v>
+        <v>0.188609191195769</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>6.619030469740215</v>
+        <v>0.188609191195769</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.779108819735061</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.990777123454038</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>3.358303226289058</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3.904777396593537</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1.644156523126431</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1.612743423246858</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1.829189117262751</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1.828540277365283</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1.995597596835747</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1.322189866823892</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1.225977001497085</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.9792252696219189</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1.186055825661855</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1.282268690988662</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1.544110198463599</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1.377052878993135</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1.204843955800101</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1.112526171453693</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1.143939271333267</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1.792507548601998</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1.544110198463599</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1.301056821126909</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1.143939271333267</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1.112526171453693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>